<commit_message>
Fixed Kpi names in template
</commit_message>
<xml_diff>
--- a/Projects/SOLARBR_SAND/Data/Score Template.xlsx
+++ b/Projects/SOLARBR_SAND/Data/Score Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="DROGARIA" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="38">
   <si>
     <t xml:space="preserve">Kpi</t>
   </si>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">SOVI STILL BALCÃO REFRIGERADO KO</t>
   </si>
   <si>
-    <t xml:space="preserve">SOVI ÁGUA </t>
+    <t xml:space="preserve">SOVI ÁGUA</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI ENERGETICO</t>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">SOVI RET Gelado KO FAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOVI ÁGUA</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI FANTA LARANJA</t>
@@ -140,34 +137,16 @@
     <t xml:space="preserve">SOVI SS SSD Seção de Bebida KO</t>
   </si>
   <si>
-    <t xml:space="preserve">SOVI SSD KO LOJA</t>
-  </si>
-  <si>
     <t xml:space="preserve">SOVI SSD KO SEÇÃO DE BEBIDAS</t>
   </si>
   <si>
-    <t xml:space="preserve">SOVI ENERGÉTICO LOJA</t>
+    <t xml:space="preserve">SOVI CCTM</t>
   </si>
   <si>
-    <t xml:space="preserve">SOVI CCTM LOJA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOVI STILL KO LOJA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOVI CERVEJA LOJA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOVI SS SSD LOJA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOVI ÁGUA KO LOJA</t>
+    <t xml:space="preserve">SOVI SS SSD</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI SSD NO CORREDOR DA FRENTE DE SEÇÃO DE BEBIDAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOVI SUCO LOJA</t>
   </si>
 </sst>
 </file>
@@ -488,25 +467,25 @@
   </sheetPr>
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.0647773279352"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1015,25 +994,25 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E69" activeCellId="0" sqref="E69"/>
+      <selection pane="topLeft" activeCell="E69" activeCellId="1" sqref="A23:A26 E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.8137651821862"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.1417004048583"/>
@@ -1193,7 +1172,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0</v>
@@ -1210,7 +1189,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.15</v>
@@ -1227,7 +1206,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0.2</v>
@@ -1244,7 +1223,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0.25</v>
@@ -1261,7 +1240,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0.3</v>
@@ -1278,7 +1257,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -1295,7 +1274,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.25</v>
@@ -1312,7 +1291,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.35</v>
@@ -1329,7 +1308,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0.45</v>
@@ -1516,7 +1495,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>0</v>
@@ -1533,7 +1512,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>0.3</v>
@@ -1558,7 +1537,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0.35</v>
@@ -1583,7 +1562,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.4</v>
@@ -1857,7 +1836,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -1874,7 +1853,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.15</v>
@@ -1891,7 +1870,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.2</v>
@@ -1908,7 +1887,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.25</v>
@@ -1925,7 +1904,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.3</v>
@@ -2027,7 +2006,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B55" s="5" t="n">
         <v>0</v>
@@ -2044,7 +2023,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56" s="5" t="n">
         <v>0.5</v>
@@ -2080,12 +2059,12 @@
   <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E67" activeCellId="0" sqref="E67"/>
+      <selection pane="topLeft" activeCell="E67" activeCellId="1" sqref="A23:A26 E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -2093,7 +2072,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -2266,7 +2245,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0</v>
@@ -2285,7 +2264,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.15</v>
@@ -2302,7 +2281,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0.2</v>
@@ -2319,7 +2298,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0.25</v>
@@ -2336,7 +2315,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0.3</v>
@@ -2353,7 +2332,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -2370,7 +2349,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.25</v>
@@ -2387,7 +2366,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.35</v>
@@ -2404,7 +2383,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0.45</v>
@@ -2591,7 +2570,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>0</v>
@@ -2608,7 +2587,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>0.3</v>
@@ -2625,7 +2604,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0.35</v>
@@ -2642,7 +2621,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.4</v>
@@ -2914,7 +2893,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -2931,7 +2910,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.15</v>
@@ -2948,7 +2927,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.2</v>
@@ -2965,7 +2944,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.25</v>
@@ -2982,7 +2961,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.3</v>
@@ -3084,7 +3063,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B55" s="5" t="n">
         <v>0</v>
@@ -3101,7 +3080,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56" s="5" t="n">
         <v>0.5</v>
@@ -3134,21 +3113,21 @@
   </sheetPr>
   <dimension ref="A1:S65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A57" activeCellId="1" sqref="A23:A26 A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -3402,7 +3381,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -3424,7 +3403,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.25</v>
@@ -3446,7 +3425,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.35</v>
@@ -3468,7 +3447,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0.45</v>
@@ -3770,7 +3749,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0</v>
@@ -3792,7 +3771,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="5" t="n">
         <v>0.5</v>
@@ -3814,7 +3793,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="5" t="n">
         <v>0</v>
@@ -3836,7 +3815,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="5" t="n">
         <v>0.15</v>
@@ -3858,7 +3837,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="5" t="n">
         <v>0.2</v>
@@ -3880,7 +3859,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="5" t="n">
         <v>0</v>
@@ -3902,7 +3881,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="5" t="n">
         <v>0.6</v>
@@ -3922,7 +3901,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" s="5" t="n">
         <v>0.66</v>
@@ -3942,7 +3921,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" s="5" t="n">
         <v>0.7</v>
@@ -3962,7 +3941,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B38" s="5" t="n">
         <v>0.75</v>
@@ -4067,7 +4046,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B44" s="5" t="n">
         <v>0</v>
@@ -4084,7 +4063,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0.25</v>
@@ -4101,7 +4080,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.3</v>
@@ -4118,7 +4097,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.35</v>
@@ -4135,7 +4114,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0</v>
@@ -4152,7 +4131,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.06</v>
@@ -4169,7 +4148,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B50" s="5" t="n">
         <v>0.07</v>
@@ -4186,7 +4165,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B51" s="5" t="n">
         <v>0.085</v>
@@ -4203,7 +4182,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B52" s="5" t="n">
         <v>0.1</v>
@@ -4305,7 +4284,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B58" s="5" t="n">
         <v>0</v>
@@ -4322,7 +4301,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B59" s="5" t="n">
         <v>0.06</v>
@@ -4339,7 +4318,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B60" s="5" t="n">
         <v>0.07</v>
@@ -4356,7 +4335,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B61" s="5" t="n">
         <v>0.085</v>
@@ -4373,7 +4352,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B62" s="5" t="n">
         <v>0.1</v>
@@ -4390,7 +4369,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B63" s="5" t="n">
         <v>0</v>
@@ -4407,7 +4386,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B64" s="5" t="n">
         <v>0.6</v>
@@ -4424,7 +4403,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B65" s="5" t="n">
         <v>0.66</v>
@@ -4441,7 +4420,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B66" s="5" t="n">
         <v>0.7</v>
@@ -4458,7 +4437,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B67" s="5" t="n">
         <v>0.75</v>
@@ -4494,12 +4473,12 @@
   <dimension ref="A1:X65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="1" sqref="A23:A26 H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -4507,7 +4486,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -4705,7 +4684,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0</v>
@@ -4735,7 +4714,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.6</v>
@@ -4765,7 +4744,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0.66</v>
@@ -4786,7 +4765,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0.7</v>
@@ -4807,7 +4786,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0.75</v>
@@ -4837,7 +4816,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -4867,7 +4846,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.25</v>
@@ -4897,7 +4876,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.3</v>
@@ -4927,7 +4906,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0.35</v>
@@ -4973,7 +4952,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>0</v>
@@ -5006,7 +4985,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>0.05</v>
@@ -5036,7 +5015,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="5" t="n">
         <v>0.15</v>
@@ -5057,7 +5036,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5" t="n">
         <v>0</v>
@@ -5078,7 +5057,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5" t="n">
         <v>0.5</v>
@@ -5393,7 +5372,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B32" s="5" t="n">
         <v>0</v>
@@ -5420,7 +5399,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B33" s="5" t="n">
         <v>0.25</v>
@@ -5450,7 +5429,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B34" s="5" t="n">
         <v>0.35</v>
@@ -5480,7 +5459,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B35" s="5" t="n">
         <v>0.45</v>
@@ -5598,7 +5577,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B39" s="5" t="n">
         <v>0</v>
@@ -5627,7 +5606,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>0.25</v>
@@ -5656,7 +5635,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" s="5" t="n">
         <v>0.3</v>
@@ -5684,7 +5663,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B42" s="5" t="n">
         <v>0.35</v>
@@ -5812,7 +5791,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0</v>
@@ -5832,7 +5811,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.15</v>
@@ -5852,7 +5831,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B50" s="5" t="n">
         <v>0.2</v>
@@ -5872,7 +5851,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B51" s="5" t="n">
         <v>0.25</v>
@@ -5889,7 +5868,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B52" s="5" t="n">
         <v>0.3</v>
@@ -5906,7 +5885,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53" s="5" t="n">
         <v>0</v>
@@ -5923,7 +5902,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" s="5" t="n">
         <v>0.25</v>
@@ -5940,7 +5919,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B55" s="5" t="n">
         <v>0.3</v>
@@ -5957,7 +5936,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B56" s="5" t="n">
         <v>0.35</v>
@@ -5974,7 +5953,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B57" s="5" t="n">
         <v>0</v>
@@ -5991,7 +5970,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B58" s="5" t="n">
         <v>0.2</v>
@@ -6008,7 +5987,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B59" s="5" t="n">
         <v>0.3</v>
@@ -6025,7 +6004,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B60" s="5" t="n">
         <v>0</v>
@@ -6042,7 +6021,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B61" s="5" t="n">
         <v>0.6</v>
@@ -6059,7 +6038,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B62" s="5" t="n">
         <v>0.66</v>
@@ -6076,7 +6055,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B63" s="5" t="n">
         <v>0.7</v>
@@ -6093,7 +6072,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B64" s="5" t="n">
         <v>0.75</v>
@@ -6280,7 +6259,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B75" s="5" t="n">
         <v>0</v>
@@ -6297,7 +6276,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B76" s="5" t="n">
         <v>0.2</v>
@@ -6314,7 +6293,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B77" s="5" t="n">
         <v>0.3</v>
@@ -6349,12 +6328,12 @@
   <dimension ref="A1:N65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E52" activeCellId="0" sqref="E52"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="1" sqref="A23:A26 A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -6362,7 +6341,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -6373,7 +6352,7 @@
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="19.7085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6402,7 +6381,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>0</v>
@@ -6424,7 +6403,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5" t="n">
         <v>0.6</v>
@@ -6446,7 +6425,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5" t="n">
         <v>0.66</v>
@@ -6465,7 +6444,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5" t="n">
         <v>0.7</v>
@@ -6482,7 +6461,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>0.75</v>
@@ -6499,7 +6478,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0</v>
@@ -6516,7 +6495,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.6</v>
@@ -6533,7 +6512,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0.66</v>
@@ -6550,7 +6529,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0.7</v>
@@ -6567,7 +6546,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0.75</v>
@@ -6584,7 +6563,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -6601,7 +6580,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.05</v>
@@ -6618,7 +6597,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.15</v>
@@ -6635,7 +6614,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0</v>
@@ -6652,7 +6631,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>0.3</v>
@@ -6669,7 +6648,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>0.33</v>
@@ -6686,7 +6665,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>0.35</v>
@@ -6710,7 +6689,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" s="5" t="n">
         <v>0.38</v>
@@ -6732,7 +6711,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="B20" s="5" t="n">
         <v>0</v>
@@ -6754,7 +6733,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="B21" s="5" t="n">
         <v>0.25</v>
@@ -6773,7 +6752,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="B22" s="5" t="n">
         <v>0.3</v>
@@ -6790,7 +6769,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="B23" s="5" t="n">
         <v>0.35</v>
@@ -6807,7 +6786,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="B24" s="5" t="n">
         <v>0.4</v>
@@ -6824,7 +6803,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B25" s="5" t="n">
         <v>0</v>
@@ -6841,7 +6820,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>0.08</v>
@@ -6858,7 +6837,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>0.13</v>
@@ -6875,7 +6854,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0</v>
@@ -6892,7 +6871,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.2</v>
@@ -6909,7 +6888,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B30" s="5" t="n">
         <v>0.33</v>
@@ -6926,7 +6905,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B31" s="5" t="n">
         <v>0</v>
@@ -6943,7 +6922,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B32" s="5" t="n">
         <v>0.25</v>
@@ -6960,7 +6939,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B33" s="5" t="n">
         <v>0.35</v>
@@ -6977,7 +6956,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B34" s="5" t="n">
         <v>0.45</v>
@@ -6994,7 +6973,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="5" t="n">
         <v>0</v>
@@ -7011,7 +6990,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" s="5" t="n">
         <v>0.6</v>
@@ -7028,7 +7007,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" s="5" t="n">
         <v>0.66</v>
@@ -7045,7 +7024,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B38" s="5" t="n">
         <v>0.7</v>
@@ -7062,7 +7041,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B39" s="5" t="n">
         <v>0.75</v>
@@ -7079,7 +7058,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>0</v>
@@ -7096,7 +7075,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B41" s="5" t="n">
         <v>0.6</v>
@@ -7113,7 +7092,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B42" s="5" t="n">
         <v>0.66</v>
@@ -7130,7 +7109,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B43" s="5" t="n">
         <v>0.7</v>
@@ -7147,7 +7126,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B44" s="5" t="n">
         <v>0.75</v>
@@ -7164,7 +7143,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -7181,7 +7160,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.25</v>
@@ -7198,7 +7177,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.3</v>
@@ -7215,7 +7194,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.35</v>
@@ -7250,19 +7229,19 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="1" sqref="A23:A26 A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
@@ -7975,12 +7954,12 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="A23:A26 E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.9271255060729"/>
@@ -7988,7 +7967,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -8291,20 +8270,20 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="1" sqref="A23:A26 E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -8605,28 +8584,28 @@
   </sheetPr>
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="1" sqref="A23:A26 A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1012145748988"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="18" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8835,7 +8814,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -8852,7 +8831,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.6</v>
@@ -8869,7 +8848,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.66</v>
@@ -8886,7 +8865,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0.7</v>
@@ -8903,7 +8882,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>0.75</v>
@@ -9158,12 +9137,12 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="1" sqref="A23:A26 G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.5587044534413"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.9878542510122"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="18" width="6.63967611336032"/>
@@ -9171,14 +9150,14 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="18" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9718,20 +9697,20 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="1" sqref="A23:A26 E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -10247,12 +10226,12 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="C32" activeCellId="1" sqref="A23:A26 C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6720647773279"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
@@ -10260,7 +10239,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -10739,12 +10718,12 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="A23:A26 A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4574898785425"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="10" width="6.63967611336032"/>
@@ -10752,7 +10731,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -11057,7 +11036,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -11080,7 +11059,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.25</v>
@@ -11103,7 +11082,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.35</v>
@@ -11126,7 +11105,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0.45</v>
@@ -11149,7 +11128,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>0</v>
@@ -11172,7 +11151,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>0.5</v>
@@ -11315,7 +11294,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="5" t="n">
         <v>0</v>
@@ -11343,7 +11322,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="5" t="n">
         <v>0.6</v>
@@ -11370,7 +11349,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="5" t="n">
         <v>0.66</v>
@@ -11397,7 +11376,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>0.7</v>
@@ -11424,7 +11403,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>0.75</v>
@@ -11451,7 +11430,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0</v>
@@ -11478,7 +11457,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.3</v>
@@ -11505,7 +11484,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" s="5" t="n">
         <v>0.35</v>
@@ -11529,7 +11508,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" s="5" t="n">
         <v>0.4</v>
@@ -11552,7 +11531,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" s="5" t="n">
         <v>0</v>
@@ -11576,7 +11555,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33" s="5" t="n">
         <v>0.6</v>
@@ -11599,7 +11578,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="5" t="n">
         <v>0.66</v>
@@ -11622,7 +11601,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="5" t="n">
         <v>0.7</v>
@@ -11645,7 +11624,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" s="5" t="n">
         <v>0.75</v>
@@ -11668,7 +11647,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" s="5" t="n">
         <v>0</v>
@@ -11691,7 +11670,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B38" s="5" t="n">
         <v>0.6</v>
@@ -11708,7 +11687,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B39" s="5" t="n">
         <v>0.66</v>
@@ -11725,7 +11704,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>0.7</v>
@@ -11742,7 +11721,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B41" s="5" t="n">
         <v>0.75</v>
@@ -11810,7 +11789,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -11827,7 +11806,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.06</v>
@@ -11844,7 +11823,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.07</v>
@@ -11861,7 +11840,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.085</v>
@@ -11878,7 +11857,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.1</v>
@@ -11980,7 +11959,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" s="5" t="n">
         <v>0</v>
@@ -11997,7 +11976,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B56" s="5" t="n">
         <v>0.3</v>
@@ -12014,7 +11993,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B57" s="5" t="n">
         <v>0.35</v>
@@ -12031,7 +12010,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B58" s="5" t="n">
         <v>0.4</v>
@@ -12048,7 +12027,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59" s="5" t="n">
         <v>0.45</v>

</xml_diff>

<commit_message>
template updatete to the beer score
</commit_message>
<xml_diff>
--- a/Projects/SOLARBR_SAND/Data/Score Template.xlsx
+++ b/Projects/SOLARBR_SAND/Data/Score Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="976" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="DROGARIA" sheetId="1" state="visible" r:id="rId2"/>
@@ -467,25 +467,25 @@
   </sheetPr>
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23:A26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.0647773279352"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3846153846154"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -994,25 +994,25 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E69" activeCellId="1" sqref="A23:A26 E69"/>
+      <selection pane="topLeft" activeCell="E69" activeCellId="0" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0283400809717"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.1417004048583"/>
@@ -2059,12 +2059,12 @@
   <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E67" activeCellId="1" sqref="A23:A26 E67"/>
+      <selection pane="topLeft" activeCell="E67" activeCellId="0" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4210526315789"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -2072,7 +2072,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -3113,21 +3113,21 @@
   </sheetPr>
   <dimension ref="A1:S65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A57" activeCellId="1" sqref="A23:A26 A57"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -3493,7 +3493,9 @@
       <c r="A17" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="0"/>
+      <c r="B17" s="22" t="n">
+        <v>0.1</v>
+      </c>
       <c r="C17" s="6" t="n">
         <v>0.1499</v>
       </c>
@@ -4473,12 +4475,12 @@
   <dimension ref="A1:X65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="1" sqref="A23:A26 H4"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -4486,7 +4488,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -6328,12 +6330,12 @@
   <dimension ref="A1:N65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="1" sqref="A23:A26 A31"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -6341,7 +6343,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -6352,7 +6354,7 @@
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="19.8178137651822"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7229,19 +7231,19 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="1" sqref="A23:A26 A20"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
@@ -7954,12 +7956,12 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="A23:A26 E17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.7085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.9271255060729"/>
@@ -7967,7 +7969,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -8270,20 +8272,20 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="1" sqref="A23:A26 E16"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -8585,27 +8587,27 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="1" sqref="A23:A26 A15"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="18" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9137,12 +9139,12 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="1" sqref="A23:A26 G10"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.9878542510122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="18" width="6.63967611336032"/>
@@ -9150,14 +9152,14 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="18" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9697,20 +9699,20 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="1" sqref="A23:A26 E26"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -10226,12 +10228,12 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="1" sqref="A23:A26 C32"/>
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8866396761134"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
@@ -10239,7 +10241,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -10718,12 +10720,12 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="A23:A26 A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6720647773279"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="10" width="6.63967611336032"/>
@@ -10731,7 +10733,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>

</xml_diff>